<commit_message>
Initialized Excel Template and Generated Scrip File
</commit_message>
<xml_diff>
--- a/dhan/src/TradeSheet.xlsx
+++ b/dhan/src/TradeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AliAsgar\Projects\excel-trading-project\dhan\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97065B-AEA6-4427-94D6-CC5DA84A1255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884B492-44F9-4CD4-9CF7-ED4F4573A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7872" yWindow="756" windowWidth="12996" windowHeight="10908" xr2:uid="{06F4B4D0-14F8-40A2-B9A2-98920E5C4291}"/>
+    <workbookView xWindow="7872" yWindow="756" windowWidth="12996" windowHeight="10908" xr2:uid="{BF0395AF-5F82-4B56-8450-529B51AE18F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Market" sheetId="3" r:id="rId1"/>
@@ -26,31 +26,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>dasd</t>
-  </si>
-  <si>
-    <t>adas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+  <si>
+    <t>Watchlist</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Buy Quntity</t>
+  </si>
+  <si>
+    <t>Buy Price</t>
+  </si>
+  <si>
+    <t>Sell Price</t>
+  </si>
+  <si>
+    <t>Sell Qauntity</t>
+  </si>
+  <si>
+    <t>Last Trade Price</t>
+  </si>
+  <si>
+    <t>Trade Station</t>
+  </si>
+  <si>
+    <t>Order Type 
+(MIS/CNC/Normal)</t>
+  </si>
+  <si>
+    <t>Buy/Sell
+(+/-)</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Trigger 
+ Price</t>
+  </si>
+  <si>
+    <t>Limit Price</t>
+  </si>
+  <si>
+    <t>Confirm?</t>
+  </si>
+  <si>
+    <t>Order management</t>
+  </si>
+  <si>
+    <t>Buy/Sell</t>
+  </si>
+  <si>
+    <t>Order Price</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Modify/Cancel</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>Trigger Price</t>
+  </si>
+  <si>
+    <t>Open Positions</t>
+  </si>
+  <si>
+    <t>Average Price</t>
+  </si>
+  <si>
+    <t>MTM 
+(Profit/Loss)</t>
+  </si>
+  <si>
+    <t>Partially
+(Quantity)</t>
+  </si>
+  <si>
+    <t>Square Off All</t>
+  </si>
+  <si>
+    <t>NSE:MARICO 25 JUL 625 CALL&amp;123483</t>
+  </si>
+  <si>
+    <t>NSE:ICICIBANK 29 AUG 1430 CALL&amp;123488</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,16 +129,334 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -75,15 +464,224 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,58 +992,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF39DE56-B912-4FE7-9888-09F56C99DCA9}">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F852244-C447-468F-9FB8-BFE2F861B713}">
+  <dimension ref="B2:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="2:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A72396D-E21D-4FD5-A7EB-12D8BAF1CC9C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45055222-A3B9-47B5-B243-A32A3E949E39}">
+  <dimension ref="B9:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="N9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="10" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="N9:T9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>